<commit_message>
added same picture 3 times for test reasons
</commit_message>
<xml_diff>
--- a/01_Paradigms/ER-ED/ER_ED/StimuliNeutral.xlsx
+++ b/01_Paradigms/ER-ED/ER_ED/StimuliNeutral.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Stimuli/083.jpg</t>
   </si>
@@ -347,24 +347,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed amount of stimuli for test purposes
</commit_message>
<xml_diff>
--- a/01_Paradigms/ER-ED/ER_ED/StimuliNeutral.xlsx
+++ b/01_Paradigms/ER-ED/ER_ED/StimuliNeutral.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scheffel\Scheffel\Forschung\A_Projects\2021_COG-ER-ED\COG-ER-ED\01_Paradigms\ER-ED\ER_ED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scheffel\Scheffel\Forschung\A_Projects\2021_CERED\CERED\01_Paradigms\ER-ED\ER_ED\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Stimuli/083.jpg</t>
   </si>
@@ -347,10 +347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,16 +368,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>